<commit_message>
Xoa lan chon truoc
</commit_message>
<xml_diff>
--- a/KTTKPM.xlsx
+++ b/KTTKPM.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\LienThong\KienTrucVaKiThuatPhanMem\res\Hg_Project\KienTrucPhanMem\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
@@ -19,8 +14,8 @@
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'DHTH8ALT '!$10:$10</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -28,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="129">
   <si>
     <t>DANH SÁCH SINH VIÊN</t>
   </si>
@@ -417,19 +412,16 @@
     <t>For a description of the “Decomposition Style”, seeDocumenting Software
 Architecture, page 53. And for an excellent discussion of the usesrelationship
 and its implications, see the same book, page 68</t>
-  </si>
-  <si>
-    <t>Chung, B.Nixon, E.Yu, J.Mylopoulos, (Editors). Non-Functional Requirements in Software Engineering Series: The Kluwer International Series in Software Engineering. Vol. 5, Kluwer Academic Publishers. 1999.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -798,9 +790,21 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="3" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -812,18 +816,6 @@
     </xf>
     <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -933,7 +925,7 @@
           <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
             <a:extLst>
               <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
               </a:ext>
             </a:extLst>
           </a:blip>
@@ -956,14 +948,14 @@
           </a:ln>
           <a:extLst>
             <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
                 <a:solidFill>
                   <a:srgbClr val="FFFFFF"/>
                 </a:solidFill>
               </a14:hiddenFill>
             </a:ext>
             <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -1236,24 +1228,24 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:H50"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D14" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A17" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.42578125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.42578125" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="5.42578125" style="2" customWidth="1"/>
     <col min="2" max="2" width="12.85546875" style="2" customWidth="1"/>
@@ -1266,7 +1258,7 @@
     <col min="9" max="16384" width="9.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="21.75" customHeight="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1275,74 +1267,74 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="40"/>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-    </row>
-    <row r="3" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="41"/>
-      <c r="B3" s="41"/>
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="41"/>
-    </row>
-    <row r="4" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="42" t="s">
+    <row r="2" spans="1:8" ht="27.75" customHeight="1">
+      <c r="A2" s="35"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+    </row>
+    <row r="3" spans="1:8" ht="22.5" customHeight="1">
+      <c r="A3" s="36"/>
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
+    </row>
+    <row r="4" spans="1:8" ht="25.5">
+      <c r="A4" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="42"/>
-      <c r="C4" s="42"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
-      <c r="G4" s="42"/>
-    </row>
-    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="35" t="s">
+      <c r="B4" s="37"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
+    </row>
+    <row r="5" spans="1:8" ht="15.75" customHeight="1">
+      <c r="B5" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="35"/>
-      <c r="D5" s="35"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
     </row>
-    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="43" t="s">
+    <row r="6" spans="1:8" ht="15.75" customHeight="1">
+      <c r="B6" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="43"/>
-      <c r="D6" s="43"/>
-    </row>
-    <row r="7" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="35" t="s">
+      <c r="C6" s="39"/>
+      <c r="D6" s="39"/>
+    </row>
+    <row r="7" spans="1:8" ht="16.5" customHeight="1">
+      <c r="B7" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="35"/>
-      <c r="D7" s="35"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
       <c r="F7" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="35" t="s">
+    <row r="8" spans="1:8" ht="16.5" customHeight="1">
+      <c r="B8" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="35"/>
-      <c r="D8" s="35"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
       <c r="E8" s="3"/>
       <c r="F8" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="13.5" customHeight="1" thickBot="1">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -1351,7 +1343,7 @@
       <c r="F9" s="21"/>
       <c r="G9" s="5"/>
     </row>
-    <row r="10" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="18.75" customHeight="1">
       <c r="A10" s="6"/>
       <c r="B10" s="7" t="s">
         <v>7</v>
@@ -1375,7 +1367,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="18.75" customHeight="1">
       <c r="A11" s="8">
         <v>1</v>
       </c>
@@ -1393,7 +1385,7 @@
       <c r="G11" s="28"/>
       <c r="H11" s="28"/>
     </row>
-    <row r="12" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="18.75" customHeight="1">
       <c r="A12" s="8">
         <v>2</v>
       </c>
@@ -1411,7 +1403,7 @@
       <c r="G12" s="28"/>
       <c r="H12" s="28"/>
     </row>
-    <row r="13" spans="1:8" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="65.25" customHeight="1">
       <c r="A13" s="8">
         <v>3</v>
       </c>
@@ -1433,7 +1425,7 @@
       </c>
       <c r="H13" s="28"/>
     </row>
-    <row r="14" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="18.75" customHeight="1">
       <c r="A14" s="8">
         <v>4</v>
       </c>
@@ -1451,7 +1443,7 @@
       <c r="G14" s="28"/>
       <c r="H14" s="28"/>
     </row>
-    <row r="15" spans="1:8" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="65.25" customHeight="1">
       <c r="A15" s="8">
         <v>5</v>
       </c>
@@ -1475,7 +1467,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="18.75" customHeight="1">
       <c r="A16" s="8">
         <v>6</v>
       </c>
@@ -1493,7 +1485,7 @@
       <c r="G16" s="28"/>
       <c r="H16" s="28"/>
     </row>
-    <row r="17" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="18.75" customHeight="1">
       <c r="A17" s="8">
         <v>7</v>
       </c>
@@ -1511,7 +1503,7 @@
       <c r="G17" s="28"/>
       <c r="H17" s="28"/>
     </row>
-    <row r="18" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="18.75" customHeight="1">
       <c r="A18" s="8">
         <v>8</v>
       </c>
@@ -1529,7 +1521,7 @@
       <c r="G18" s="28"/>
       <c r="H18" s="28"/>
     </row>
-    <row r="19" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="18.75" customHeight="1">
       <c r="A19" s="8">
         <v>9</v>
       </c>
@@ -1547,7 +1539,7 @@
       <c r="G19" s="28"/>
       <c r="H19" s="28"/>
     </row>
-    <row r="20" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="18.75" customHeight="1">
       <c r="A20" s="8">
         <v>10</v>
       </c>
@@ -1565,7 +1557,7 @@
       <c r="G20" s="28"/>
       <c r="H20" s="28"/>
     </row>
-    <row r="21" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="18.75" customHeight="1">
       <c r="A21" s="8">
         <v>11</v>
       </c>
@@ -1583,7 +1575,7 @@
       <c r="G21" s="28"/>
       <c r="H21" s="28"/>
     </row>
-    <row r="22" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="18.75" customHeight="1">
       <c r="A22" s="8">
         <v>12</v>
       </c>
@@ -1601,7 +1593,7 @@
       <c r="G22" s="28"/>
       <c r="H22" s="28"/>
     </row>
-    <row r="23" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="18.75" customHeight="1">
       <c r="A23" s="8">
         <v>13</v>
       </c>
@@ -1619,7 +1611,7 @@
       <c r="G23" s="28"/>
       <c r="H23" s="28"/>
     </row>
-    <row r="24" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="18.75" customHeight="1">
       <c r="A24" s="8">
         <v>14</v>
       </c>
@@ -1637,7 +1629,7 @@
       <c r="G24" s="28"/>
       <c r="H24" s="28"/>
     </row>
-    <row r="25" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="18.75" customHeight="1">
       <c r="A25" s="8">
         <v>15</v>
       </c>
@@ -1651,15 +1643,11 @@
         <v>53</v>
       </c>
       <c r="E25" s="25"/>
-      <c r="F25" s="34" t="s">
-        <v>125</v>
-      </c>
-      <c r="G25" s="34" t="s">
-        <v>129</v>
-      </c>
+      <c r="F25" s="34"/>
+      <c r="G25" s="34"/>
       <c r="H25" s="28"/>
     </row>
-    <row r="26" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="18.75" customHeight="1">
       <c r="A26" s="8">
         <v>16</v>
       </c>
@@ -1677,7 +1665,7 @@
       <c r="G26" s="28"/>
       <c r="H26" s="28"/>
     </row>
-    <row r="27" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="18.75" customHeight="1">
       <c r="A27" s="8">
         <v>17</v>
       </c>
@@ -1695,7 +1683,7 @@
       <c r="G27" s="28"/>
       <c r="H27" s="28"/>
     </row>
-    <row r="28" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="18.75" customHeight="1">
       <c r="A28" s="8">
         <v>18</v>
       </c>
@@ -1713,7 +1701,7 @@
       <c r="G28" s="28"/>
       <c r="H28" s="28"/>
     </row>
-    <row r="29" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="18.75" customHeight="1">
       <c r="A29" s="8">
         <v>19</v>
       </c>
@@ -1731,7 +1719,7 @@
       <c r="G29" s="28"/>
       <c r="H29" s="28"/>
     </row>
-    <row r="30" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" ht="18.75" customHeight="1">
       <c r="A30" s="8">
         <v>20</v>
       </c>
@@ -1749,7 +1737,7 @@
       <c r="G30" s="28"/>
       <c r="H30" s="28"/>
     </row>
-    <row r="31" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="18.75" customHeight="1">
       <c r="A31" s="8">
         <v>21</v>
       </c>
@@ -1767,7 +1755,7 @@
       <c r="G31" s="28"/>
       <c r="H31" s="28"/>
     </row>
-    <row r="32" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" ht="18.75" customHeight="1">
       <c r="A32" s="8">
         <v>22</v>
       </c>
@@ -1785,7 +1773,7 @@
       <c r="G32" s="28"/>
       <c r="H32" s="28"/>
     </row>
-    <row r="33" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" ht="18.75" customHeight="1">
       <c r="A33" s="8">
         <v>23</v>
       </c>
@@ -1803,7 +1791,7 @@
       <c r="G33" s="28"/>
       <c r="H33" s="28"/>
     </row>
-    <row r="34" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" ht="18.75" customHeight="1">
       <c r="A34" s="8">
         <v>24</v>
       </c>
@@ -1821,7 +1809,7 @@
       <c r="G34" s="28"/>
       <c r="H34" s="28"/>
     </row>
-    <row r="35" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" ht="18.75" customHeight="1">
       <c r="A35" s="8">
         <v>25</v>
       </c>
@@ -1839,7 +1827,7 @@
       <c r="G35" s="28"/>
       <c r="H35" s="28"/>
     </row>
-    <row r="36" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" ht="18.75" customHeight="1">
       <c r="A36" s="8">
         <v>26</v>
       </c>
@@ -1857,7 +1845,7 @@
       <c r="G36" s="28"/>
       <c r="H36" s="28"/>
     </row>
-    <row r="37" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" ht="18.75" customHeight="1">
       <c r="A37" s="8">
         <v>27</v>
       </c>
@@ -1875,7 +1863,7 @@
       <c r="G37" s="28"/>
       <c r="H37" s="28"/>
     </row>
-    <row r="38" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" ht="18.75" customHeight="1">
       <c r="A38" s="8">
         <v>28</v>
       </c>
@@ -1893,7 +1881,7 @@
       <c r="G38" s="28"/>
       <c r="H38" s="28"/>
     </row>
-    <row r="39" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" ht="18.75" customHeight="1">
       <c r="A39" s="8">
         <v>29</v>
       </c>
@@ -1911,7 +1899,7 @@
       <c r="G39" s="28"/>
       <c r="H39" s="28"/>
     </row>
-    <row r="40" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" ht="18.75" customHeight="1">
       <c r="A40" s="8">
         <v>30</v>
       </c>
@@ -1929,7 +1917,7 @@
       <c r="G40" s="28"/>
       <c r="H40" s="28"/>
     </row>
-    <row r="41" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" ht="18.75" customHeight="1">
       <c r="A41" s="8">
         <v>31</v>
       </c>
@@ -1947,7 +1935,7 @@
       <c r="G41" s="28"/>
       <c r="H41" s="28"/>
     </row>
-    <row r="42" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" ht="18.75" customHeight="1">
       <c r="A42" s="8">
         <v>32</v>
       </c>
@@ -1965,7 +1953,7 @@
       <c r="G42" s="28"/>
       <c r="H42" s="28"/>
     </row>
-    <row r="43" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" ht="18.75" customHeight="1">
       <c r="A43" s="8">
         <v>33</v>
       </c>
@@ -1983,7 +1971,7 @@
       <c r="G43" s="28"/>
       <c r="H43" s="28"/>
     </row>
-    <row r="44" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" ht="18.75" customHeight="1">
       <c r="A44" s="8">
         <v>34</v>
       </c>
@@ -2001,7 +1989,7 @@
       <c r="G44" s="28"/>
       <c r="H44" s="28"/>
     </row>
-    <row r="45" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" ht="18.75" customHeight="1">
       <c r="A45" s="8">
         <v>35</v>
       </c>
@@ -2025,7 +2013,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" ht="18.75" customHeight="1">
       <c r="A46" s="8">
         <v>36</v>
       </c>
@@ -2043,7 +2031,7 @@
       <c r="G46" s="28"/>
       <c r="H46" s="28"/>
     </row>
-    <row r="47" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" ht="18.75" customHeight="1">
       <c r="A47" s="8">
         <v>37</v>
       </c>
@@ -2059,27 +2047,27 @@
       <c r="G47" s="28"/>
       <c r="H47" s="28"/>
     </row>
-    <row r="48" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="36" t="s">
+    <row r="48" spans="1:8" ht="18" thickBot="1">
+      <c r="A48" s="40" t="s">
         <v>116</v>
       </c>
-      <c r="B48" s="37"/>
-      <c r="C48" s="37"/>
-      <c r="D48" s="38"/>
+      <c r="B48" s="41"/>
+      <c r="C48" s="41"/>
+      <c r="D48" s="42"/>
       <c r="E48" s="18"/>
       <c r="F48" s="18"/>
       <c r="G48" s="18"/>
       <c r="H48" s="22"/>
     </row>
-    <row r="49" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A49" s="39"/>
-      <c r="B49" s="39"/>
-      <c r="C49" s="39"/>
+    <row r="49" spans="1:4" ht="17.25">
+      <c r="A49" s="43"/>
+      <c r="B49" s="43"/>
+      <c r="C49" s="43"/>
       <c r="D49" s="15" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" ht="15.75" customHeight="1">
       <c r="A50" s="16"/>
       <c r="B50" s="17"/>
       <c r="C50" s="17"/>
@@ -2087,16 +2075,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="A49:C49"/>
+    <mergeCell ref="B7:D7"/>
     <mergeCell ref="A2:G2"/>
     <mergeCell ref="A3:G3"/>
     <mergeCell ref="A4:G4"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="A49:C49"/>
-    <mergeCell ref="B7:D7"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>

</xml_diff>

<commit_message>
Da dang ky bao thu hoach - Ngo Quoc Hung - hehe
</commit_message>
<xml_diff>
--- a/KTTKPM.xlsx
+++ b/KTTKPM.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="131">
   <si>
     <t>DANH SÁCH SINH VIÊN</t>
   </si>
@@ -412,6 +412,14 @@
     <t>For a description of the “Decomposition Style”, seeDocumenting Software
 Architecture, page 53. And for an excellent discussion of the usesrelationship
 and its implications, see the same book, page 68</t>
+  </si>
+  <si>
+    <t>4.7.1 CORBA</t>
+  </si>
+  <si>
+    <t>http://www.omg.org, A New Approach to Object-Oriented Middleware”
+(IEEE Internet Computing, Jan 2004) and The Rise and Fall of CORBA (ACM
+Queue, Jun 2006)</t>
   </si>
 </sst>
 </file>
@@ -702,7 +710,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -790,6 +798,21 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -799,23 +822,11 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -925,7 +936,7 @@
           <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
             <a:extLst>
               <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+                <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
               </a:ext>
             </a:extLst>
           </a:blip>
@@ -948,14 +959,14 @@
           </a:ln>
           <a:extLst>
             <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+              <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
                 <a:solidFill>
                   <a:srgbClr val="FFFFFF"/>
                 </a:solidFill>
               </a14:hiddenFill>
             </a:ext>
             <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
+              <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -1228,7 +1239,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1241,8 +1252,8 @@
   </sheetPr>
   <dimension ref="A1:H50"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A17" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D11" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.42578125" defaultRowHeight="15.75"/>
@@ -1268,67 +1279,67 @@
       <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:8" ht="27.75" customHeight="1">
-      <c r="A2" s="35"/>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
+      <c r="A2" s="40"/>
+      <c r="B2" s="40"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
     </row>
     <row r="3" spans="1:8" ht="22.5" customHeight="1">
-      <c r="A3" s="36"/>
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36"/>
+      <c r="A3" s="41"/>
+      <c r="B3" s="41"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
     </row>
     <row r="4" spans="1:8" ht="25.5">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="37"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
+      <c r="B4" s="42"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="42"/>
     </row>
     <row r="5" spans="1:8" ht="15.75" customHeight="1">
-      <c r="B5" s="38" t="s">
+      <c r="B5" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="38"/>
-      <c r="D5" s="38"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="35"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
     </row>
     <row r="6" spans="1:8" ht="15.75" customHeight="1">
-      <c r="B6" s="39" t="s">
+      <c r="B6" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="43"/>
     </row>
     <row r="7" spans="1:8" ht="16.5" customHeight="1">
-      <c r="B7" s="38" t="s">
+      <c r="B7" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="38"/>
-      <c r="D7" s="38"/>
+      <c r="C7" s="35"/>
+      <c r="D7" s="35"/>
       <c r="F7" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="16.5" customHeight="1">
-      <c r="B8" s="38" t="s">
+      <c r="B8" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="38"/>
-      <c r="D8" s="38"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="35"/>
       <c r="E8" s="3"/>
       <c r="F8" s="4" t="s">
         <v>6</v>
@@ -1629,7 +1640,7 @@
       <c r="G24" s="28"/>
       <c r="H24" s="28"/>
     </row>
-    <row r="25" spans="1:8" ht="18.75" customHeight="1">
+    <row r="25" spans="1:8" ht="46.5" customHeight="1">
       <c r="A25" s="8">
         <v>15</v>
       </c>
@@ -1643,8 +1654,12 @@
         <v>53</v>
       </c>
       <c r="E25" s="25"/>
-      <c r="F25" s="34"/>
-      <c r="G25" s="34"/>
+      <c r="F25" s="34" t="s">
+        <v>129</v>
+      </c>
+      <c r="G25" s="44" t="s">
+        <v>130</v>
+      </c>
       <c r="H25" s="28"/>
     </row>
     <row r="26" spans="1:8" ht="18.75" customHeight="1">
@@ -2048,21 +2063,21 @@
       <c r="H47" s="28"/>
     </row>
     <row r="48" spans="1:8" ht="18" thickBot="1">
-      <c r="A48" s="40" t="s">
+      <c r="A48" s="36" t="s">
         <v>116</v>
       </c>
-      <c r="B48" s="41"/>
-      <c r="C48" s="41"/>
-      <c r="D48" s="42"/>
+      <c r="B48" s="37"/>
+      <c r="C48" s="37"/>
+      <c r="D48" s="38"/>
       <c r="E48" s="18"/>
       <c r="F48" s="18"/>
       <c r="G48" s="18"/>
       <c r="H48" s="22"/>
     </row>
     <row r="49" spans="1:4" ht="17.25">
-      <c r="A49" s="43"/>
-      <c r="B49" s="43"/>
-      <c r="C49" s="43"/>
+      <c r="A49" s="39"/>
+      <c r="B49" s="39"/>
+      <c r="C49" s="39"/>
       <c r="D49" s="15" t="s">
         <v>117</v>
       </c>
@@ -2075,16 +2090,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B6:D6"/>
     <mergeCell ref="B8:D8"/>
     <mergeCell ref="A48:B48"/>
     <mergeCell ref="C48:D48"/>
     <mergeCell ref="A49:C49"/>
     <mergeCell ref="B7:D7"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B6:D6"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>

</xml_diff>